<commit_message>
use 0611 version benchmark report
</commit_message>
<xml_diff>
--- a/lib/report/benchmark_report/web14/exl/201903/jsliu__bank_test_&_city_(HF)(201903)_Two_Cycles_Comparison.xlsx
+++ b/lib/report/benchmark_report/web14/exl/201903/jsliu__bank_test_&_city_(HF)(201903)_Two_Cycles_Comparison.xlsx
@@ -347,7 +347,7 @@
     <t xml:space="preserve">Bank Name: jsliu  bank test &amp; city (HF)</t>
   </si>
   <si>
-    <t>Printed on: 05/21/19 2:23:07PM</t>
+    <t>Printed on: 06/11/19 4:53:06AM</t>
   </si>
   <si>
     <t xml:space="preserve"> Rate Shock</t>
@@ -745,7 +745,7 @@
     </r>
   </si>
   <si>
-    <t>Printed on: 05/21/19 2:23:02PM</t>
+    <t>Printed on: 06/11/19 4:53:00AM</t>
   </si>
   <si>
     <t xml:space="preserve">Earning/
@@ -4078,13 +4078,13 @@
       <c r="N23" s="96"/>
       <c r="O23" s="96"/>
       <c r="P23" s="96">
-        <v>160.61500026090823</v>
+        <v>158.98276607032085</v>
       </c>
       <c r="Q23" s="96"/>
       <c r="R23" s="96"/>
       <c r="S23" s="96"/>
       <c r="T23" s="96">
-        <v>43.589077072965729</v>
+        <v>-3.896255466083034</v>
       </c>
       <c r="U23" s="96"/>
       <c r="V23" s="96"/>
@@ -4106,7 +4106,7 @@
       <c r="AL23" s="96"/>
       <c r="AM23" s="96"/>
       <c r="AN23" s="96">
-        <v>-78.628974097538176</v>
+        <v>-29.511407367902024</v>
       </c>
       <c r="AO23" s="96"/>
       <c r="AP23" s="96"/>
@@ -4136,13 +4136,13 @@
       <c r="N24" s="96"/>
       <c r="O24" s="96"/>
       <c r="P24" s="96">
-        <v>321.23000052181646</v>
+        <v>317.9655321406417</v>
       </c>
       <c r="Q24" s="96"/>
       <c r="R24" s="96"/>
       <c r="S24" s="96"/>
       <c r="T24" s="96">
-        <v>87.178154145931458</v>
+        <v>-7.7925109321660679</v>
       </c>
       <c r="U24" s="96"/>
       <c r="V24" s="96"/>
@@ -4164,7 +4164,7 @@
       <c r="AL24" s="96"/>
       <c r="AM24" s="96"/>
       <c r="AN24" s="96">
-        <v>-462.34097519491968</v>
+        <v>-364.10584173564735</v>
       </c>
       <c r="AO24" s="96"/>
       <c r="AP24" s="96"/>
@@ -4194,13 +4194,13 @@
       <c r="N25" s="96"/>
       <c r="O25" s="96"/>
       <c r="P25" s="96">
-        <v>160.61500026090823</v>
+        <v>158.98276607032085</v>
       </c>
       <c r="Q25" s="96"/>
       <c r="R25" s="96"/>
       <c r="S25" s="96"/>
       <c r="T25" s="96">
-        <v>43.589077072965729</v>
+        <v>-3.896255466083034</v>
       </c>
       <c r="U25" s="96"/>
       <c r="V25" s="96"/>
@@ -4228,7 +4228,7 @@
       <c r="AL25" s="96"/>
       <c r="AM25" s="96"/>
       <c r="AN25" s="96">
-        <v>-78.62897409753802</v>
+        <v>-29.511407367901871</v>
       </c>
       <c r="AO25" s="96"/>
       <c r="AP25" s="96"/>
@@ -4258,13 +4258,13 @@
       <c r="N26" s="96"/>
       <c r="O26" s="96"/>
       <c r="P26" s="96">
-        <v>321.23000052181646</v>
+        <v>317.9655321406417</v>
       </c>
       <c r="Q26" s="96"/>
       <c r="R26" s="96"/>
       <c r="S26" s="96"/>
       <c r="T26" s="96">
-        <v>87.178154145931458</v>
+        <v>-7.7925109321660679</v>
       </c>
       <c r="U26" s="96"/>
       <c r="V26" s="96"/>
@@ -4292,7 +4292,7 @@
       <c r="AL26" s="96"/>
       <c r="AM26" s="96"/>
       <c r="AN26" s="96">
-        <v>-462.34097519491746</v>
+        <v>-364.10584173564519</v>
       </c>
       <c r="AO26" s="96"/>
       <c r="AP26" s="96"/>
@@ -4892,7 +4892,7 @@
       <c r="T38" s="142"/>
       <c r="U38" s="142"/>
       <c r="V38" s="142">
-        <v>5.17480343124657</v>
+        <v>5.12055109949589</v>
       </c>
       <c r="W38" s="142"/>
       <c r="X38" s="142">
@@ -4943,7 +4943,7 @@
         <v>0.034650779812070133</v>
       </c>
       <c r="AW38" s="144">
-        <v>0.030637367598148266</v>
+        <v>0.02036695293029047</v>
       </c>
       <c r="AX38" s="144">
         <v>-0.00866354875647155</v>
@@ -4996,7 +4996,7 @@
       <c r="T39" s="142"/>
       <c r="U39" s="142"/>
       <c r="V39" s="142">
-        <v>5.17480343124657</v>
+        <v>5.12055109949589</v>
       </c>
       <c r="W39" s="142"/>
       <c r="X39" s="142">
@@ -5047,7 +5047,7 @@
         <v>0.034650779812070133</v>
       </c>
       <c r="AW39" s="144">
-        <v>0.030637367598148266</v>
+        <v>0.02036695293029047</v>
       </c>
       <c r="AX39" s="144">
         <v>-0.00866354875647155</v>
@@ -5100,7 +5100,7 @@
       <c r="T40" s="142"/>
       <c r="U40" s="142"/>
       <c r="V40" s="142">
-        <v>0.738026476033199</v>
+        <v>0.728732572593343</v>
       </c>
       <c r="W40" s="142"/>
       <c r="X40" s="142">
@@ -5151,7 +5151,7 @@
         <v>0.036196626884559158</v>
       </c>
       <c r="AW40" s="144">
-        <v>0.17748819165180552</v>
+        <v>0.16699827311045978</v>
       </c>
       <c r="AX40" s="144">
         <v>0.0064462990583165989</v>
@@ -5204,7 +5204,7 @@
       <c r="T41" s="142"/>
       <c r="U41" s="142"/>
       <c r="V41" s="142">
-        <v>3.16703699542729</v>
+        <v>39.9338023176773</v>
       </c>
       <c r="W41" s="142"/>
       <c r="X41" s="142">
@@ -5255,7 +5255,7 @@
         <v>0.022397094430992737</v>
       </c>
       <c r="AW41" s="144">
-        <v>0.041139253670000681</v>
+        <v>0.9239554642722847</v>
       </c>
       <c r="AX41" s="144">
         <v>-0.072408594312293739</v>
@@ -5572,7 +5572,7 @@
       <c r="T46" s="146"/>
       <c r="U46" s="146"/>
       <c r="V46" s="146">
-        <v>0.639206112071918</v>
+        <v>0.639219398340249</v>
       </c>
       <c r="W46" s="146"/>
       <c r="X46" s="146">
@@ -5623,7 +5623,7 @@
         <v>0.12534578146611342</v>
       </c>
       <c r="AW46" s="148">
-        <v>-0.14475392032493364</v>
+        <v>-0.14473012644790512</v>
       </c>
       <c r="AX46" s="148">
         <v>1.1443750425221118E-05</v>
@@ -5988,7 +5988,7 @@
       <c r="T50" s="138"/>
       <c r="U50" s="138"/>
       <c r="V50" s="138">
-        <v>2.67103277887751</v>
+        <v>2.66947742611074</v>
       </c>
       <c r="W50" s="138"/>
       <c r="X50" s="138">
@@ -6039,7 +6039,7 @@
         <v>-0.028555111364934323</v>
       </c>
       <c r="AW50" s="140">
-        <v>-0.031544798456508892</v>
+        <v>-0.032145820978982075</v>
       </c>
       <c r="AX50" s="140">
         <v>0.034628241204863824</v>
@@ -6092,7 +6092,7 @@
       <c r="T51" s="146"/>
       <c r="U51" s="146"/>
       <c r="V51" s="146">
-        <v>2.67103277887751</v>
+        <v>2.66947742611074</v>
       </c>
       <c r="W51" s="146"/>
       <c r="X51" s="146">
@@ -6143,7 +6143,7 @@
         <v>-0.028555111364934323</v>
       </c>
       <c r="AW51" s="148">
-        <v>-0.031544798456508892</v>
+        <v>-0.032145820978982075</v>
       </c>
       <c r="AX51" s="148">
         <v>0.034628241204863824</v>
@@ -6404,7 +6404,7 @@
       <c r="T54" s="146"/>
       <c r="U54" s="146"/>
       <c r="V54" s="146">
-        <v>2.46365800097372</v>
+        <v>2.44821092276747</v>
       </c>
       <c r="W54" s="146"/>
       <c r="X54" s="146">
@@ -6455,7 +6455,7 @@
         <v>-0.034369114877589452</v>
       </c>
       <c r="AW54" s="148">
-        <v>-0.021748682074753421</v>
+        <v>-0.028195443525070075</v>
       </c>
       <c r="AX54" s="148">
         <v>0.033868213156182152</v>
@@ -6508,7 +6508,7 @@
       <c r="T55" s="146"/>
       <c r="U55" s="146"/>
       <c r="V55" s="146">
-        <v>2.05528512665803</v>
+        <v>2.04899777285687</v>
       </c>
       <c r="W55" s="146"/>
       <c r="X55" s="146">
@@ -6559,7 +6559,7 @@
         <v>-0.0022271714922048975</v>
       </c>
       <c r="AW55" s="148">
-        <v>-0.040555819876260488</v>
+        <v>-0.043748767509530086</v>
       </c>
       <c r="AX55" s="148">
         <v>0.017884479672408291</v>
@@ -7370,7 +7370,7 @@
       </c>
       <c r="U63" s="146"/>
       <c r="V63" s="146">
-        <v>6.09415919484274</v>
+        <v>6.09382977776269</v>
       </c>
       <c r="W63" s="146"/>
       <c r="X63" s="146">
@@ -7423,7 +7423,7 @@
         <v>0.024567481357865607</v>
       </c>
       <c r="AW63" s="148">
-        <v>0.048358791193839873</v>
+        <v>0.048307347868428392</v>
       </c>
       <c r="AX63" s="148">
         <v>-0.027590049405365021</v>
@@ -7478,7 +7478,7 @@
       </c>
       <c r="U64" s="146"/>
       <c r="V64" s="146">
-        <v>6.12655254061217</v>
+        <v>6.12543724070776</v>
       </c>
       <c r="W64" s="146"/>
       <c r="X64" s="146">
@@ -7531,7 +7531,7 @@
         <v>0.021150248108679735</v>
       </c>
       <c r="AW64" s="148">
-        <v>0.0484481081998788</v>
+        <v>0.048274852693004425</v>
       </c>
       <c r="AX64" s="148">
         <v>-0.026356462707333075</v>
@@ -7910,7 +7910,7 @@
       </c>
       <c r="U68" s="146"/>
       <c r="V68" s="146">
-        <v>6.03491151832635</v>
+        <v>6.02218700476174</v>
       </c>
       <c r="W68" s="146"/>
       <c r="X68" s="146">
@@ -7963,7 +7963,7 @@
         <v>0.030735706448860173</v>
       </c>
       <c r="AW68" s="148">
-        <v>0.041499874975788539</v>
+        <v>0.039474622715620071</v>
       </c>
       <c r="AX68" s="148">
         <v>-0.01838037231825617</v>
@@ -8666,7 +8666,7 @@
       </c>
       <c r="U75" s="146"/>
       <c r="V75" s="146">
-        <v>6.26113992116509</v>
+        <v>6.24402359516556</v>
       </c>
       <c r="W75" s="146"/>
       <c r="X75" s="146">
@@ -8719,7 +8719,7 @@
         <v>0.02776777398323502</v>
       </c>
       <c r="AW75" s="148">
-        <v>0.044483414973275785</v>
+        <v>0.0418641210007261</v>
       </c>
       <c r="AX75" s="148">
         <v>-0.012574012203512437</v>
@@ -9292,7 +9292,7 @@
       <c r="T81" s="146"/>
       <c r="U81" s="146"/>
       <c r="V81" s="146">
-        <v>5.17480343124657</v>
+        <v>5.12055109949589</v>
       </c>
       <c r="W81" s="146"/>
       <c r="X81" s="146">
@@ -9343,7 +9343,7 @@
         <v>0.034650779812070133</v>
       </c>
       <c r="AW81" s="148">
-        <v>0.030637367598148266</v>
+        <v>0.02036695293029047</v>
       </c>
       <c r="AX81" s="148">
         <v>-0.00866354875647155</v>
@@ -9452,7 +9452,7 @@
       <c r="T84" s="138"/>
       <c r="U84" s="138"/>
       <c r="V84" s="138">
-        <v>1.37579311311981</v>
+        <v>1.37479121160142</v>
       </c>
       <c r="W84" s="138"/>
       <c r="X84" s="138">
@@ -9503,7 +9503,7 @@
         <v>0.013201850186303482</v>
       </c>
       <c r="AW84" s="140">
-        <v>0.26400332514344388</v>
+        <v>0.26346695556248784</v>
       </c>
       <c r="AX84" s="140">
         <v>0.0053165733159862335</v>
@@ -9880,7 +9880,7 @@
       <c r="T88" s="146"/>
       <c r="U88" s="146"/>
       <c r="V88" s="146">
-        <v>0.740805717347044</v>
+        <v>0.73136550756921</v>
       </c>
       <c r="W88" s="146"/>
       <c r="X88" s="146">
@@ -9931,7 +9931,7 @@
         <v>0.036009897521240258</v>
       </c>
       <c r="AW88" s="148">
-        <v>0.17763523869528231</v>
+        <v>0.16702044242683747</v>
       </c>
       <c r="AX88" s="148">
         <v>0.0064611321032391113</v>
@@ -10192,7 +10192,7 @@
       <c r="T91" s="146"/>
       <c r="U91" s="146"/>
       <c r="V91" s="146">
-        <v>0.738026476033199</v>
+        <v>0.728732572593343</v>
       </c>
       <c r="W91" s="146"/>
       <c r="X91" s="146">
@@ -10243,7 +10243,7 @@
         <v>0.036196626884559158</v>
       </c>
       <c r="AW91" s="148">
-        <v>0.17748819165180552</v>
+        <v>0.16699827311045978</v>
       </c>
       <c r="AX91" s="148">
         <v>0.0064462990583165989</v>
@@ -10352,7 +10352,7 @@
       <c r="T94" s="146"/>
       <c r="U94" s="146"/>
       <c r="V94" s="146">
-        <v>3.16703699542729</v>
+        <v>39.9338023176773</v>
       </c>
       <c r="W94" s="146"/>
       <c r="X94" s="146">
@@ -10403,7 +10403,7 @@
         <v>0.022397094430992737</v>
       </c>
       <c r="AW94" s="148">
-        <v>0.041139253670000681</v>
+        <v>0.9239554642722847</v>
       </c>
       <c r="AX94" s="148">
         <v>-0.072408594312293739</v>
@@ -30750,16 +30750,16 @@
         <v>125.57510323633579</v>
       </c>
       <c r="F22" s="49">
-        <v>160.61500026090823</v>
+        <v>158.98276607032085</v>
       </c>
       <c r="G22" s="49">
-        <v>43.589077072965729</v>
+        <v>-3.896255466083034</v>
       </c>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
       <c r="J22" s="49"/>
       <c r="K22" s="49">
-        <v>-78.628974097538176</v>
+        <v>-29.511407367902024</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -30776,16 +30776,16 @@
         <v>-53.932820527171714</v>
       </c>
       <c r="F23" s="49">
-        <v>321.23000052181646</v>
+        <v>317.9655321406417</v>
       </c>
       <c r="G23" s="49">
-        <v>87.178154145931458</v>
+        <v>-7.7925109321660679</v>
       </c>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
       <c r="J23" s="49"/>
       <c r="K23" s="49">
-        <v>-462.34097519491968</v>
+        <v>-364.10584173564735</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -30802,10 +30802,10 @@
         <v>65.9025647577871</v>
       </c>
       <c r="F24" s="49">
-        <v>160.61500026090823</v>
+        <v>158.98276607032085</v>
       </c>
       <c r="G24" s="49">
-        <v>43.589077072965729</v>
+        <v>-3.896255466083034</v>
       </c>
       <c r="H24" s="49">
         <v>-177</v>
@@ -30817,7 +30817,7 @@
         <v>1.3274615214516088</v>
       </c>
       <c r="K24" s="49">
-        <v>-78.62897409753802</v>
+        <v>-29.511407367901871</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
@@ -30834,10 +30834,10 @@
         <v>-134.54879736187846</v>
       </c>
       <c r="F25" s="49">
-        <v>321.23000052181646</v>
+        <v>317.9655321406417</v>
       </c>
       <c r="G25" s="49">
-        <v>87.178154145931458</v>
+        <v>-7.7925109321660679</v>
       </c>
       <c r="H25" s="49">
         <v>-354</v>
@@ -30849,7 +30849,7 @@
         <v>41.384023165291808</v>
       </c>
       <c r="K25" s="49">
-        <v>-462.34097519491746</v>
+        <v>-364.10584173564519</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
@@ -35222,7 +35222,7 @@
       </c>
       <c r="J10" s="169"/>
       <c r="K10" s="169">
-        <v>5.17480343124657</v>
+        <v>5.12055109949589</v>
       </c>
       <c r="L10" s="169">
         <v>16.0520191649555</v>
@@ -35259,7 +35259,7 @@
         <v>0.034650779812070133</v>
       </c>
       <c r="X10" s="171">
-        <v>0.030637367598148266</v>
+        <v>0.02036695293029047</v>
       </c>
       <c r="Y10" s="171">
         <v>-0.00866354875647155</v>
@@ -35301,7 +35301,7 @@
       </c>
       <c r="J11" s="169"/>
       <c r="K11" s="169">
-        <v>5.17480343124657</v>
+        <v>5.12055109949589</v>
       </c>
       <c r="L11" s="169">
         <v>16.0520191649555</v>
@@ -35338,7 +35338,7 @@
         <v>0.034650779812070133</v>
       </c>
       <c r="X11" s="171">
-        <v>0.030637367598148266</v>
+        <v>0.02036695293029047</v>
       </c>
       <c r="Y11" s="171">
         <v>-0.00866354875647155</v>
@@ -35380,7 +35380,7 @@
       </c>
       <c r="J12" s="169"/>
       <c r="K12" s="169">
-        <v>0.738026476033199</v>
+        <v>0.728732572593343</v>
       </c>
       <c r="L12" s="169">
         <v>0.966461327857632</v>
@@ -35417,7 +35417,7 @@
         <v>0.036196626884559158</v>
       </c>
       <c r="X12" s="171">
-        <v>0.17748819165180552</v>
+        <v>0.16699827311045978</v>
       </c>
       <c r="Y12" s="171">
         <v>0.0064462990583165989</v>
@@ -35459,7 +35459,7 @@
       </c>
       <c r="J13" s="169"/>
       <c r="K13" s="169">
-        <v>3.16703699542729</v>
+        <v>39.9338023176773</v>
       </c>
       <c r="L13" s="169">
         <v>12.6160164271047</v>
@@ -35496,7 +35496,7 @@
         <v>0.022397094430992737</v>
       </c>
       <c r="X13" s="171">
-        <v>0.041139253670000681</v>
+        <v>0.9239554642722847</v>
       </c>
       <c r="Y13" s="171">
         <v>-0.072408594312293739</v>
@@ -35728,7 +35728,7 @@
       </c>
       <c r="J18" s="173"/>
       <c r="K18" s="173">
-        <v>0.639206112071918</v>
+        <v>0.639219398340249</v>
       </c>
       <c r="L18" s="173">
         <v>0.0219028062970568</v>
@@ -35765,7 +35765,7 @@
         <v>0.12534578146611342</v>
       </c>
       <c r="X18" s="175">
-        <v>-0.14475392032493364</v>
+        <v>-0.14473012644790512</v>
       </c>
       <c r="Y18" s="175">
         <v>1.1443750425221118E-05</v>
@@ -36044,7 +36044,7 @@
       </c>
       <c r="J22" s="165"/>
       <c r="K22" s="165">
-        <v>2.67103277887751</v>
+        <v>2.66947742611074</v>
       </c>
       <c r="L22" s="165">
         <v>24.5776865160849</v>
@@ -36081,7 +36081,7 @@
         <v>-0.028555111364934323</v>
       </c>
       <c r="X22" s="167">
-        <v>-0.031544798456508892</v>
+        <v>-0.032145820978982075</v>
       </c>
       <c r="Y22" s="167">
         <v>0.034628241204863824</v>
@@ -36123,7 +36123,7 @@
       </c>
       <c r="J23" s="173"/>
       <c r="K23" s="173">
-        <v>2.67103277887751</v>
+        <v>2.66947742611074</v>
       </c>
       <c r="L23" s="173">
         <v>24.5776865160849</v>
@@ -36160,7 +36160,7 @@
         <v>-0.028555111364934323</v>
       </c>
       <c r="X23" s="175">
-        <v>-0.031544798456508892</v>
+        <v>-0.032145820978982075</v>
       </c>
       <c r="Y23" s="175">
         <v>0.034628241204863824</v>
@@ -36360,7 +36360,7 @@
       </c>
       <c r="J26" s="173"/>
       <c r="K26" s="173">
-        <v>2.46365800097372</v>
+        <v>2.44821092276747</v>
       </c>
       <c r="L26" s="173">
         <v>21.5085557837098</v>
@@ -36397,7 +36397,7 @@
         <v>-0.034369114877589452</v>
       </c>
       <c r="X26" s="175">
-        <v>-0.021748682074753421</v>
+        <v>-0.028195443525070075</v>
       </c>
       <c r="Y26" s="175">
         <v>0.033868213156182152</v>
@@ -36439,7 +36439,7 @@
       </c>
       <c r="J27" s="173"/>
       <c r="K27" s="173">
-        <v>2.05528512665803</v>
+        <v>2.04899777285687</v>
       </c>
       <c r="L27" s="173">
         <v>9.72210814510609</v>
@@ -36476,7 +36476,7 @@
         <v>-0.0022271714922048975</v>
       </c>
       <c r="X27" s="175">
-        <v>-0.040555819876260488</v>
+        <v>-0.043748767509530086</v>
       </c>
       <c r="Y27" s="175">
         <v>0.017884479672408291</v>
@@ -37101,7 +37101,7 @@
         <v>21.934912442203743</v>
       </c>
       <c r="K35" s="173">
-        <v>6.09415919484274</v>
+        <v>6.09382977776269</v>
       </c>
       <c r="L35" s="173">
         <v>29.700205338809</v>
@@ -37140,7 +37140,7 @@
         <v>0.024567481357865607</v>
       </c>
       <c r="X35" s="175">
-        <v>0.048358791193839873</v>
+        <v>0.048307347868428392</v>
       </c>
       <c r="Y35" s="175">
         <v>-0.027590049405365021</v>
@@ -37184,7 +37184,7 @@
         <v>22.059458908516579</v>
       </c>
       <c r="K36" s="173">
-        <v>6.12655254061217</v>
+        <v>6.12543724070776</v>
       </c>
       <c r="L36" s="173">
         <v>28.9472963723477</v>
@@ -37223,7 +37223,7 @@
         <v>0.021150248108679735</v>
       </c>
       <c r="X36" s="175">
-        <v>0.0484481081998788</v>
+        <v>0.048274852693004425</v>
       </c>
       <c r="Y36" s="175">
         <v>-0.026356462707333075</v>
@@ -37516,7 +37516,7 @@
         <v>16.692594780208466</v>
       </c>
       <c r="K40" s="173">
-        <v>6.03491151832635</v>
+        <v>6.02218700476174</v>
       </c>
       <c r="L40" s="173">
         <v>22.4339493497604</v>
@@ -37555,7 +37555,7 @@
         <v>0.030735706448860173</v>
       </c>
       <c r="X40" s="175">
-        <v>0.041499874975788539</v>
+        <v>0.039474622715620071</v>
       </c>
       <c r="Y40" s="175">
         <v>-0.01838037231825617</v>
@@ -38097,7 +38097,7 @@
         <v>14.91025113965819</v>
       </c>
       <c r="K47" s="173">
-        <v>6.26113992116509</v>
+        <v>6.24402359516556</v>
       </c>
       <c r="L47" s="173">
         <v>18.9295003422314</v>
@@ -38136,7 +38136,7 @@
         <v>0.02776777398323502</v>
       </c>
       <c r="X47" s="175">
-        <v>0.044483414973275785</v>
+        <v>0.0418641210007261</v>
       </c>
       <c r="Y47" s="175">
         <v>-0.012574012203512437</v>
@@ -38573,7 +38573,7 @@
       </c>
       <c r="J53" s="173"/>
       <c r="K53" s="173">
-        <v>5.17480343124657</v>
+        <v>5.12055109949589</v>
       </c>
       <c r="L53" s="173">
         <v>16.0520191649555</v>
@@ -38610,7 +38610,7 @@
         <v>0.034650779812070133</v>
       </c>
       <c r="X53" s="175">
-        <v>0.030637367598148266</v>
+        <v>0.02036695293029047</v>
       </c>
       <c r="Y53" s="175">
         <v>-0.00866354875647155</v>
@@ -38684,7 +38684,7 @@
       </c>
       <c r="J56" s="165"/>
       <c r="K56" s="165">
-        <v>1.37579311311981</v>
+        <v>1.37479121160142</v>
       </c>
       <c r="L56" s="165">
         <v>0.966461327857632</v>
@@ -38721,7 +38721,7 @@
         <v>0.013201850186303482</v>
       </c>
       <c r="X56" s="167">
-        <v>0.26400332514344388</v>
+        <v>0.26346695556248784</v>
       </c>
       <c r="Y56" s="167">
         <v>0.0053165733159862335</v>
@@ -39012,7 +39012,7 @@
       </c>
       <c r="J60" s="173"/>
       <c r="K60" s="173">
-        <v>0.740805717347044</v>
+        <v>0.73136550756921</v>
       </c>
       <c r="L60" s="173">
         <v>0.966461327857632</v>
@@ -39049,7 +39049,7 @@
         <v>0.036009897521240258</v>
       </c>
       <c r="X60" s="175">
-        <v>0.17763523869528231</v>
+        <v>0.16702044242683747</v>
       </c>
       <c r="Y60" s="175">
         <v>0.0064611321032391113</v>
@@ -39249,7 +39249,7 @@
       </c>
       <c r="J63" s="173"/>
       <c r="K63" s="173">
-        <v>0.738026476033199</v>
+        <v>0.728732572593343</v>
       </c>
       <c r="L63" s="173">
         <v>0.966461327857632</v>
@@ -39286,7 +39286,7 @@
         <v>0.036196626884559158</v>
       </c>
       <c r="X63" s="175">
-        <v>0.17748819165180552</v>
+        <v>0.16699827311045978</v>
       </c>
       <c r="Y63" s="175">
         <v>0.0064462990583165989</v>
@@ -39360,7 +39360,7 @@
       </c>
       <c r="J66" s="173"/>
       <c r="K66" s="173">
-        <v>3.16703699542729</v>
+        <v>39.9338023176773</v>
       </c>
       <c r="L66" s="173">
         <v>12.6160164271047</v>
@@ -39397,7 +39397,7 @@
         <v>0.022397094430992737</v>
       </c>
       <c r="X66" s="175">
-        <v>0.041139253670000681</v>
+        <v>0.9239554642722847</v>
       </c>
       <c r="Y66" s="175">
         <v>-0.072408594312293739</v>

</xml_diff>